<commit_message>
created some more tests on heatmaps
</commit_message>
<xml_diff>
--- a/SocialNodework/Genetico/gen-johnson8-2-4.clqc.xlsx
+++ b/SocialNodework/Genetico/gen-johnson8-2-4.clqc.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Potato\source\repos\luisccgoncalves\SocialNodework\SocialNodework\Genetico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23EF7588-59DA-494B-8C2E-DB75CF2B95DB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{65890633-F82A-4E27-A4E0-BC403878C4D2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gen-johnson8-2-4.clqc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -862,7 +862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CZ106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">

</xml_diff>